<commit_message>
Made the qualification organization contained.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-bc-practitioner.xlsx
+++ b/docs/StructureDefinition-bc-practitioner.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$50</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="319">
   <si>
     <t>Path</t>
   </si>
@@ -303,10 +303,46 @@
     <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again. Contained resources may have profiles and tags In their meta elements, but SHALL NOT have security labels.</t>
   </si>
   <si>
+    <t xml:space="preserve">type:$this}
+</t>
+  </si>
+  <si>
+    <t>The organization that authorized a qualification.</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
     <t>DomainResource.contained</t>
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>QualificationOrganization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organization {http://hl7.org/fhir/ca-bc/provider/StructureDefinition/bc-organization}
+</t>
+  </si>
+  <si>
+    <t>A grouping of people or organizations with a common purpose</t>
+  </si>
+  <si>
+    <t>A formally or informally recognized grouping of people or organizations formed for the purpose of achieving some form of collective action.  Includes companies, institutions, corporations, departments, community groups, healthcare practice groups, payer/insurer, etc.</t>
+  </si>
+  <si>
+    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}org-1:The organization SHALL at least have a name or an identifier, and possibly more than one {(identifier.count() + name.count()) &gt; 0}</t>
+  </si>
+  <si>
+    <t>(also see master files messages)</t>
+  </si>
+  <si>
+    <t>Organization(classCode=ORG, determinerCode=INST)</t>
+  </si>
+  <si>
+    <t>Organization</t>
   </si>
   <si>
     <t>Practitioner.extension</t>
@@ -324,9 +360,6 @@
   <si>
     <t xml:space="preserve">value:url}
 </t>
-  </si>
-  <si>
-    <t>open</t>
   </si>
   <si>
     <t>DomainResource.extension</t>
@@ -1134,7 +1167,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM49"/>
+  <dimension ref="A1:AM50"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1144,7 +1177,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="39.5703125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="23.33203125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="23.8515625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
@@ -1170,7 +1203,7 @@
     <col min="25" max="25" width="54.953125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="44.22265625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
@@ -2037,19 +2070,19 @@
         <v>40</v>
       </c>
       <c r="AA8" t="s" s="2">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="AB8" t="s" s="2">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="AC8" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD8" t="s" s="2">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>41</v>
@@ -2067,7 +2100,7 @@
         <v>40</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AL8" t="s" s="2">
         <v>40</v>
@@ -2076,23 +2109,25 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" hidden="true">
+    <row r="9">
       <c r="A9" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>97</v>
+      </c>
       <c r="C9" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s" s="2">
         <v>42</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s" s="2">
         <v>40</v>
@@ -2101,15 +2136,17 @@
         <v>40</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="M9" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="M9" t="s" s="2">
+        <v>91</v>
+      </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
         <v>40</v>
@@ -2146,17 +2183,19 @@
         <v>40</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AB9" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AB9" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="AC9" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>41</v>
@@ -2171,25 +2210,23 @@
         <v>101</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="AL9" t="s" s="2">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="AM9" t="s" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>102</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
         <v>40</v>
       </c>
@@ -2198,10 +2235,10 @@
         <v>50</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H10" t="s" s="2">
         <v>40</v>
@@ -2210,13 +2247,13 @@
         <v>40</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -2255,19 +2292,17 @@
         <v>40</v>
       </c>
       <c r="AA10" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB10" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="AB10" s="2"/>
       <c r="AC10" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD10" t="s" s="2">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>41</v>
@@ -2276,10 +2311,10 @@
         <v>42</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>40</v>
@@ -2296,17 +2331,17 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C11" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>50</v>
@@ -2321,13 +2356,13 @@
         <v>40</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2378,7 +2413,7 @@
         <v>40</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>41</v>
@@ -2387,10 +2422,10 @@
         <v>42</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>40</v>
@@ -2407,10 +2442,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s" s="2">
         <v>40</v>
@@ -2420,7 +2455,7 @@
         <v>41</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>51</v>
@@ -2432,13 +2467,13 @@
         <v>40</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -2489,7 +2524,7 @@
         <v>40</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>41</v>
@@ -2498,10 +2533,10 @@
         <v>42</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ12" t="s" s="2">
         <v>40</v>
@@ -2518,10 +2553,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s" s="2">
         <v>40</v>
@@ -2531,7 +2566,7 @@
         <v>41</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>51</v>
@@ -2543,13 +2578,13 @@
         <v>40</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2600,7 +2635,7 @@
         <v>40</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>41</v>
@@ -2609,10 +2644,10 @@
         <v>42</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ13" t="s" s="2">
         <v>40</v>
@@ -2629,10 +2664,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C14" t="s" s="2">
         <v>40</v>
@@ -2654,13 +2689,13 @@
         <v>40</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2711,7 +2746,7 @@
         <v>40</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>41</v>
@@ -2720,10 +2755,10 @@
         <v>42</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ14" t="s" s="2">
         <v>40</v>
@@ -2740,10 +2775,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C15" t="s" s="2">
         <v>40</v>
@@ -2765,13 +2800,13 @@
         <v>40</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2822,7 +2857,7 @@
         <v>40</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>41</v>
@@ -2831,10 +2866,10 @@
         <v>42</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ15" t="s" s="2">
         <v>40</v>
@@ -2851,10 +2886,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C16" t="s" s="2">
         <v>40</v>
@@ -2864,7 +2899,7 @@
         <v>41</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>51</v>
@@ -2876,13 +2911,13 @@
         <v>40</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2933,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>41</v>
@@ -2942,10 +2977,10 @@
         <v>42</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ16" t="s" s="2">
         <v>40</v>
@@ -2962,10 +2997,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s" s="2">
         <v>40</v>
@@ -2987,13 +3022,13 @@
         <v>40</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -3044,7 +3079,7 @@
         <v>40</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -3053,10 +3088,10 @@
         <v>42</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ17" t="s" s="2">
         <v>40</v>
@@ -3073,10 +3108,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>40</v>
@@ -3098,13 +3133,13 @@
         <v>40</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3155,7 +3190,7 @@
         <v>40</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>41</v>
@@ -3164,10 +3199,10 @@
         <v>42</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ18" t="s" s="2">
         <v>40</v>
@@ -3184,10 +3219,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C19" t="s" s="2">
         <v>40</v>
@@ -3209,13 +3244,13 @@
         <v>40</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3266,7 +3301,7 @@
         <v>40</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>41</v>
@@ -3275,10 +3310,10 @@
         <v>42</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ19" t="s" s="2">
         <v>40</v>
@@ -3293,13 +3328,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" hidden="true">
+    <row r="20">
       <c r="A20" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="B20" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>149</v>
+      </c>
       <c r="C20" t="s" s="2">
-        <v>144</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3309,29 +3346,25 @@
         <v>42</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I20" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>148</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>40</v>
       </c>
@@ -3379,7 +3412,7 @@
         <v>40</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>149</v>
+        <v>110</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>41</v>
@@ -3388,16 +3421,16 @@
         <v>42</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ20" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>40</v>
@@ -3406,42 +3439,44 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>42</v>
       </c>
       <c r="G21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H21" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="H21" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="I21" t="s" s="2">
         <v>40</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>151</v>
+        <v>106</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="M21" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="M21" t="s" s="2">
+        <v>157</v>
+      </c>
       <c r="N21" t="s" s="2">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>40</v>
@@ -3490,7 +3525,7 @@
         <v>40</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>41</v>
@@ -3499,19 +3534,19 @@
         <v>42</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>155</v>
+        <v>40</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>157</v>
+        <v>40</v>
       </c>
       <c r="AM21" t="s" s="2">
         <v>40</v>
@@ -3519,7 +3554,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3527,10 +3562,10 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>51</v>
@@ -3539,102 +3574,98 @@
         <v>40</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="L22" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="O22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P22" s="2"/>
+      <c r="Q22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE22" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="L22" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="O22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P22" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="Q22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE22" t="s" s="2">
-        <v>158</v>
-      </c>
       <c r="AF22" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>62</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>166</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3642,10 +3673,10 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F23" t="s" s="2">
         <v>50</v>
-      </c>
-      <c r="F23" t="s" s="2">
-        <v>42</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>51</v>
@@ -3654,100 +3685,102 @@
         <v>40</v>
       </c>
       <c r="I23" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="K23" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="L23" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="N23" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="O23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P23" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="Q23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE23" t="s" s="2">
         <v>168</v>
       </c>
-      <c r="K23" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="L23" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="O23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="P23" s="2"/>
-      <c r="Q23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="R23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE23" t="s" s="2">
-        <v>167</v>
-      </c>
       <c r="AF23" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>62</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>173</v>
+        <v>40</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>40</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3755,7 +3788,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F24" t="s" s="2">
         <v>42</v>
@@ -3770,19 +3803,19 @@
         <v>40</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>40</v>
@@ -3831,7 +3864,7 @@
         <v>40</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>41</v>
@@ -3840,10 +3873,10 @@
         <v>42</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>182</v>
+        <v>62</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>183</v>
@@ -3953,19 +3986,19 @@
         <v>42</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>62</v>
+        <v>192</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>40</v>
@@ -3973,7 +4006,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3984,7 +4017,7 @@
         <v>41</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>51</v>
@@ -3993,20 +4026,22 @@
         <v>40</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>70</v>
+        <v>197</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="M26" s="2"/>
+        <v>199</v>
+      </c>
+      <c r="M26" t="s" s="2">
+        <v>200</v>
+      </c>
       <c r="N26" t="s" s="2">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>40</v>
@@ -4031,13 +4066,13 @@
         <v>40</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>199</v>
+        <v>40</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>201</v>
+        <v>40</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>40</v>
@@ -4055,16 +4090,16 @@
         <v>40</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>62</v>
@@ -4107,17 +4142,17 @@
         <v>51</v>
       </c>
       <c r="J27" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K27" t="s" s="2">
         <v>206</v>
       </c>
-      <c r="K27" t="s" s="2">
+      <c r="L27" t="s" s="2">
         <v>207</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>208</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" t="s" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>40</v>
@@ -4142,13 +4177,13 @@
         <v>40</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>40</v>
+        <v>209</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>40</v>
+        <v>210</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>40</v>
+        <v>211</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>40</v>
@@ -4181,21 +4216,21 @@
         <v>62</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="28" hidden="true">
+    <row r="28">
       <c r="A28" t="s" s="2">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4209,25 +4244,27 @@
         <v>50</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="I28" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>52</v>
+        <v>216</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="N28" t="s" s="2">
+        <v>219</v>
+      </c>
       <c r="O28" t="s" s="2">
         <v>40</v>
       </c>
@@ -4275,7 +4312,7 @@
         <v>40</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>41</v>
@@ -4287,16 +4324,16 @@
         <v>40</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>40</v>
+        <v>220</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>40</v>
+        <v>221</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>40</v>
+        <v>222</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>40</v>
@@ -4304,7 +4341,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4315,7 +4352,7 @@
         <v>41</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>40</v>
@@ -4327,13 +4364,13 @@
         <v>40</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>96</v>
+        <v>224</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>97</v>
+        <v>225</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4372,29 +4409,31 @@
         <v>40</v>
       </c>
       <c r="AA29" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AB29" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="AC29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD29" t="s" s="2">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>40</v>
@@ -4409,13 +4448,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="B30" t="s" s="2">
-        <v>219</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
         <v>40</v>
       </c>
@@ -4424,10 +4461,10 @@
         <v>41</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>40</v>
@@ -4436,13 +4473,13 @@
         <v>40</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>220</v>
+        <v>106</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>221</v>
+        <v>107</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>222</v>
+        <v>108</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -4481,19 +4518,17 @@
         <v>40</v>
       </c>
       <c r="AA30" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB30" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="AB30" s="2"/>
       <c r="AC30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD30" t="s" s="2">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -4502,10 +4537,10 @@
         <v>42</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>40</v>
@@ -4520,11 +4555,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" hidden="true">
+    <row r="31">
       <c r="A31" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="B31" s="2"/>
+        <v>227</v>
+      </c>
+      <c r="B31" t="s" s="2">
+        <v>229</v>
+      </c>
       <c r="C31" t="s" s="2">
         <v>40</v>
       </c>
@@ -4536,7 +4573,7 @@
         <v>50</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>40</v>
@@ -4545,13 +4582,13 @@
         <v>40</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -4602,19 +4639,19 @@
         <v>40</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>40</v>
@@ -4631,7 +4668,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4642,7 +4679,7 @@
         <v>41</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>40</v>
@@ -4654,18 +4691,16 @@
         <v>40</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="M32" s="2"/>
-      <c r="N32" t="s" s="2">
-        <v>231</v>
-      </c>
+      <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
         <v>40</v>
       </c>
@@ -4713,36 +4748,36 @@
         <v>40</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>232</v>
+        <v>40</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>233</v>
+        <v>40</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4756,7 +4791,7 @@
         <v>42</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>40</v>
@@ -4765,16 +4800,18 @@
         <v>40</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="N33" t="s" s="2">
+        <v>241</v>
+      </c>
       <c r="O33" t="s" s="2">
         <v>40</v>
       </c>
@@ -4822,7 +4859,7 @@
         <v>40</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>41</v>
@@ -4837,21 +4874,21 @@
         <v>62</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>238</v>
+        <v>40</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="34" hidden="true">
+    <row r="34">
       <c r="A34" t="s" s="2">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4862,10 +4899,10 @@
         <v>41</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>40</v>
@@ -4874,13 +4911,13 @@
         <v>40</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>52</v>
+        <v>245</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -4931,28 +4968,28 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>40</v>
+        <v>248</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>40</v>
@@ -4960,7 +4997,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4968,11 +5005,11 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F35" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="F35" t="s" s="2">
-        <v>42</v>
-      </c>
       <c r="G35" t="s" s="2">
         <v>40</v>
       </c>
@@ -4983,13 +5020,13 @@
         <v>40</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>96</v>
+        <v>252</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>97</v>
+        <v>253</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5028,35 +5065,37 @@
         <v>40</v>
       </c>
       <c r="AA35" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AB35" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="AB35" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="AC35" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD35" t="s" s="2">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH35" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>40</v>
+        <v>254</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>40</v>
@@ -5065,13 +5104,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="B36" t="s" s="2">
-        <v>246</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
         <v>40</v>
       </c>
@@ -5080,10 +5117,10 @@
         <v>50</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>40</v>
@@ -5092,13 +5129,13 @@
         <v>40</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>247</v>
+        <v>106</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>248</v>
+        <v>107</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>249</v>
+        <v>108</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5137,19 +5174,17 @@
         <v>40</v>
       </c>
       <c r="AA36" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB36" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="AB36" s="2"/>
       <c r="AC36" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD36" t="s" s="2">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
@@ -5158,10 +5193,10 @@
         <v>42</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>40</v>
@@ -5178,17 +5213,17 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C37" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F37" t="s" s="2">
         <v>50</v>
@@ -5203,13 +5238,13 @@
         <v>40</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>108</v>
+        <v>257</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>109</v>
+        <v>258</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>110</v>
+        <v>259</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5260,7 +5295,7 @@
         <v>40</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -5269,10 +5304,10 @@
         <v>42</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>40</v>
@@ -5287,45 +5322,43 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" hidden="true">
+    <row r="38">
       <c r="A38" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="B38" s="2"/>
+        <v>255</v>
+      </c>
+      <c r="B38" t="s" s="2">
+        <v>260</v>
+      </c>
       <c r="C38" t="s" s="2">
-        <v>252</v>
+        <v>40</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>253</v>
+        <v>119</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>148</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>40</v>
       </c>
@@ -5373,7 +5406,7 @@
         <v>40</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>255</v>
+        <v>228</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -5382,16 +5415,16 @@
         <v>42</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>40</v>
@@ -5400,13 +5433,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -5416,26 +5449,28 @@
         <v>42</v>
       </c>
       <c r="G39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H39" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="H39" t="s" s="2">
-        <v>40</v>
-      </c>
       <c r="I39" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>257</v>
+        <v>106</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="M39" s="2"/>
+        <v>264</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>157</v>
+      </c>
       <c r="N39" t="s" s="2">
-        <v>260</v>
+        <v>158</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>40</v>
@@ -5484,7 +5519,7 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -5496,13 +5531,13 @@
         <v>40</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>261</v>
+        <v>96</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>40</v>
@@ -5513,7 +5548,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5521,10 +5556,10 @@
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>51</v>
@@ -5536,16 +5571,18 @@
         <v>40</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="N40" t="s" s="2">
+        <v>270</v>
+      </c>
       <c r="O40" t="s" s="2">
         <v>40</v>
       </c>
@@ -5569,35 +5606,37 @@
         <v>40</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="X40" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="X40" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="Y40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE40" t="s" s="2">
         <v>266</v>
       </c>
-      <c r="Z40" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA40" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB40" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>262</v>
-      </c>
       <c r="AF40" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>40</v>
@@ -5609,10 +5648,10 @@
         <v>40</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>239</v>
+        <v>271</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>267</v>
+        <v>40</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>40</v>
@@ -5620,7 +5659,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5628,7 +5667,7 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F41" t="s" s="2">
         <v>50</v>
@@ -5643,18 +5682,16 @@
         <v>40</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="M41" s="2"/>
-      <c r="N41" t="s" s="2">
-        <v>272</v>
-      </c>
+      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>40</v>
       </c>
@@ -5678,13 +5715,11 @@
         <v>40</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="X41" s="2"/>
       <c r="Y41" t="s" s="2">
-        <v>40</v>
+        <v>276</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>40</v>
@@ -5702,10 +5737,10 @@
         <v>40</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>50</v>
@@ -5720,10 +5755,10 @@
         <v>40</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>40</v>
@@ -5731,7 +5766,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5754,16 +5789,18 @@
         <v>40</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
+      <c r="N42" t="s" s="2">
+        <v>282</v>
+      </c>
       <c r="O42" t="s" s="2">
         <v>40</v>
       </c>
@@ -5811,7 +5848,7 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
@@ -5829,10 +5866,10 @@
         <v>40</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>40</v>
+        <v>284</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>40</v>
@@ -5840,7 +5877,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5851,7 +5888,7 @@
         <v>41</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>51</v>
@@ -5863,20 +5900,16 @@
         <v>40</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>263</v>
+        <v>286</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>284</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>40</v>
       </c>
@@ -5900,13 +5933,13 @@
         <v>40</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>40</v>
@@ -5924,13 +5957,13 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>40</v>
@@ -5939,21 +5972,21 @@
         <v>62</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>285</v>
+        <v>40</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>287</v>
+        <v>40</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="44" hidden="true">
+    <row r="44">
       <c r="A44" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -5964,10 +5997,10 @@
         <v>41</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>40</v>
@@ -5976,16 +6009,20 @@
         <v>40</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>52</v>
+        <v>273</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>242</v>
+        <v>291</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+        <v>292</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>294</v>
+      </c>
       <c r="O44" t="s" s="2">
         <v>40</v>
       </c>
@@ -6009,13 +6046,13 @@
         <v>40</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>40</v>
@@ -6033,28 +6070,28 @@
         <v>40</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>216</v>
+        <v>290</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>40</v>
+        <v>295</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>244</v>
+        <v>296</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>40</v>
+        <v>297</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>40</v>
@@ -6062,7 +6099,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6070,11 +6107,11 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F45" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="F45" t="s" s="2">
-        <v>42</v>
-      </c>
       <c r="G45" t="s" s="2">
         <v>40</v>
       </c>
@@ -6085,13 +6122,13 @@
         <v>40</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>96</v>
+        <v>252</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>97</v>
+        <v>253</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6130,37 +6167,37 @@
         <v>40</v>
       </c>
       <c r="AA45" t="s" s="2">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="AB45" t="s" s="2">
-        <v>290</v>
+        <v>40</v>
       </c>
       <c r="AC45" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD45" t="s" s="2">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>40</v>
+        <v>254</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>40</v>
@@ -6169,13 +6206,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="B46" t="s" s="2">
-        <v>291</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
         <v>40</v>
       </c>
@@ -6184,10 +6219,10 @@
         <v>50</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>40</v>
@@ -6196,13 +6231,13 @@
         <v>40</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6241,19 +6276,19 @@
         <v>40</v>
       </c>
       <c r="AA46" t="s" s="2">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="AB46" t="s" s="2">
-        <v>40</v>
+        <v>300</v>
       </c>
       <c r="AC46" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AD46" t="s" s="2">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -6265,7 +6300,7 @@
         <v>40</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>40</v>
@@ -6282,17 +6317,17 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="C47" t="s" s="2">
         <v>40</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F47" t="s" s="2">
         <v>50</v>
@@ -6307,13 +6342,13 @@
         <v>40</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6364,7 +6399,7 @@
         <v>40</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6376,7 +6411,7 @@
         <v>40</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>40</v>
@@ -6391,11 +6426,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" hidden="true">
+    <row r="48">
       <c r="A48" t="s" s="2">
-        <v>292</v>
-      </c>
-      <c r="B48" s="2"/>
+        <v>299</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>260</v>
+      </c>
       <c r="C48" t="s" s="2">
         <v>40</v>
       </c>
@@ -6404,32 +6441,28 @@
         <v>41</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>40</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>293</v>
+        <v>118</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>294</v>
+        <v>119</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>297</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>40</v>
       </c>
@@ -6477,7 +6510,7 @@
         <v>40</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>298</v>
+        <v>228</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
@@ -6489,13 +6522,13 @@
         <v>40</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>299</v>
+        <v>40</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>300</v>
+        <v>40</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>40</v>
@@ -6506,7 +6539,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6517,7 +6550,7 @@
         <v>41</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>40</v>
@@ -6529,19 +6562,19 @@
         <v>51</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>52</v>
+        <v>303</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>40</v>
@@ -6590,13 +6623,13 @@
         <v>40</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>40</v>
@@ -6605,20 +6638,133 @@
         <v>62</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM49" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" hidden="true">
+      <c r="A50" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F50" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I50" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J50" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="K50" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="O50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P50" s="2"/>
+      <c r="Q50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE50" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="AF50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG50" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI50" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="AJ50" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="AK50" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="AL50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM50" t="s" s="2">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM49">
+  <autoFilter ref="A1:AM50">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -6628,7 +6774,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI48">
+  <conditionalFormatting sqref="A2:AI49">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>